<commit_message>
updated notebooks to use redefined collect_text_content_bs()
</commit_message>
<xml_diff>
--- a/data_etl_scripts/Rules On Contracting Arrangement data.xlsx
+++ b/data_etl_scripts/Rules On Contracting Arrangement data.xlsx
@@ -1,48 +1,482 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mig\Desktop\projects\RS_for_labor_related_cases\data_etl_scripts\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>link_text</t>
-  </si>
-  <si>
-    <t>page_link</t>
-  </si>
-  <si>
-    <t>page_header</t>
-  </si>
-  <si>
-    <t>page_text_content</t>
-  </si>
-  <si>
-    <t>Department Order No. 18-02, (Series of 2002) [Rules Implementing Articles 106 to 109 of the Labor Code, as Amended]</t>
-  </si>
-  <si>
-    <t>https://www.chanrobles.com/doledepartmentorderno18-02-2002.html</t>
-  </si>
-  <si>
-    <t>DEPARTMENT ORDER NO. 18 - 02 (Series of 2002) RULES IMPLEMENTING ARTICLES 106 TO 109 OF THE LABOR CODE, AS AMENDED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
+</styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>link_text</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>page_link</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>page_header</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>page_text_content</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Department Order No. 18-02, (Series of 2002) [Rules Implementing Articles 106 to 109 of the Labor Code, as Amended]</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://www.chanrobles.com/doledepartmentorderno18-02-2002.html</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>DEPARTMENT ORDER NO. 18 - 02 (Series of 2002) RULES IMPLEMENTING ARTICLES 106 TO 109 OF THE LABOR CODE, AS AMENDED</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
 By virtue of the
         power vested in the Secretary of Labor and Employment under Articles 5
         (Rule-making) and 106 (Contractor or Subcontractor) of the Labor
@@ -597,18 +1031,31 @@
         its
         publication in two (2) newspapers of general circulation.
 </t>
-  </si>
-  <si>
-    <t>Department Order No. 3, (Series of 2001) [Revoking Department Order No. 10, Series of 1997, and Continuing to Prohibit Labor-Only Contracting]</t>
-  </si>
-  <si>
-    <t>https://www.chanrobles.com/doledepartmentorderno03-2001.html</t>
-  </si>
-  <si>
-    <t>DEPARTMENT ORDER NO. 03 (Series of 2001) REVOKING DEPARTMENT ORDER NO. 10, SERIES OF 1997, AND CONTINUING TO PROHIBIT LABOR-ONLY CONTRACTING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Department Order No. 3, (Series of 2001) [Revoking Department Order No. 10, Series of 1997, and Continuing to Prohibit Labor-Only Contracting]</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://www.chanrobles.com/doledepartmentorderno03-2001.html</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>DEPARTMENT ORDER NO. 03 (Series of 2001) REVOKING DEPARTMENT ORDER NO. 10, SERIES OF 1997, AND CONTINUING TO PROHIBIT LABOR-ONLY CONTRACTING</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
 This web page
 features
 the full text of
@@ -720,18 +1167,31 @@
 to Philippine Labor Circular Index
  chanroblesvirtualawlibrary
 </t>
-  </si>
-  <si>
-    <t>DOLE Primer on Contracting and Subcontracting Under Articles 106 to 109 of the Labor Code</t>
-  </si>
-  <si>
-    <t>https://www.chanrobles.com/dolecontractingsubcontractingprimer.html</t>
-  </si>
-  <si>
-    <t>DOLE PRIMER ON CONTRACTING AND SUBCONTRACTING Effects of Department Order No. 3, Series of 2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>DOLE Primer on Contracting and Subcontracting Under Articles 106 to 109 of the Labor Code</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://www.chanrobles.com/dolecontractingsubcontractingprimer.html</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>DOLE PRIMER ON CONTRACTING AND SUBCONTRACTING Effects of Department Order No. 3, Series of 2001</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
 1. WHAT IS CONTRACTING
 AND SUBCONTRACTING?
 There
@@ -1243,18 +1703,31 @@
 49,
 series of 1998.
 </t>
-  </si>
-  <si>
-    <t>Department Order No. 10, (Series of 1997) [Amending the Rules Implementing Books III and VI of the Labor Code, as Amended]</t>
-  </si>
-  <si>
-    <t>https://www.chanrobles.com/doledepartmentorderno10-1997.htm</t>
-  </si>
-  <si>
-    <t>DEPARTMENT ORDER NO. 10 (Series of 1997) AMENDING THE RULES IMPLEMENTING BOOKS III AND VI OF THE LABOR CODE, AS AMENDED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Department Order No. 10, (Series of 1997) [Amending the Rules Implementing Books III and VI of the Labor Code, as Amended]</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://www.chanrobles.com/doledepartmentorderno10-1997.htm</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>DEPARTMENT ORDER NO. 10 (Series of 1997) AMENDING THE RULES IMPLEMENTING BOOKS III AND VI OF THE LABOR CODE, AS AMENDED</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
 This web page
 features
 the full text of
@@ -2204,465 +2677,7 @@
 to Philippine Labor Circular Index
  chanroblesvirtualawlibrary
 </t>
-  </si>
-</sst>
-</file>
-
-<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>